<commit_message>
[Fix]: update tuning data with 3 networks (DeepLabV3, DeepLabV3+, PAN)
</commit_message>
<xml_diff>
--- a/eval/tuning/configs_best.xlsx
+++ b/eval/tuning/configs_best.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O34"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1574,11 +1574,11 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>38</v>
+        <v>434</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>dark-sweep-389</t>
+          <t>pretty-sweep-24</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1587,7 +1587,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>1971</v>
+        <v>7004</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
@@ -1596,48 +1596,48 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>FPN</t>
+          <t>DeepLabV3</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>resnet101</t>
+          <t>resnet50</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>512</v>
+        <v>896</v>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>RMSprop</t>
+          <t>Adam</t>
         </is>
       </c>
       <c r="J20" t="n">
         <v>1e-05</v>
       </c>
       <c r="K20" t="n">
-        <v>0.9885302484035492</v>
+        <v>0.988914430141449</v>
       </c>
       <c r="L20" t="n">
-        <v>0.9774056673049928</v>
+        <v>0.9781160652637479</v>
       </c>
       <c r="M20" t="n">
-        <v>0.9924060702323914</v>
+        <v>0.990272849798202</v>
       </c>
       <c r="N20" t="n">
-        <v>0.9880223870277404</v>
+        <v>0.991412878036499</v>
       </c>
       <c r="O20" t="n">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>174</v>
+        <v>388</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>wobbly-sweep-323</t>
+          <t>splendid-sweep-70</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1646,7 +1646,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>4797</v>
+        <v>3559</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
@@ -1655,36 +1655,36 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>LinkNet</t>
+          <t>DeepLabV3Plus</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>efficientnet-b5</t>
+          <t>resnet101</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>640</v>
+        <v>512</v>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>RAdam</t>
+          <t>RMSprop</t>
         </is>
       </c>
       <c r="J21" t="n">
-        <v>0.0001</v>
+        <v>1e-05</v>
       </c>
       <c r="K21" t="n">
-        <v>0.9884950816631316</v>
+        <v>0.988765001296997</v>
       </c>
       <c r="L21" t="n">
-        <v>0.9772969484329224</v>
+        <v>0.97782814502716</v>
       </c>
       <c r="M21" t="n">
-        <v>0.9928045868873596</v>
+        <v>0.990845054388046</v>
       </c>
       <c r="N21" t="n">
-        <v>0.9911109209060668</v>
+        <v>0.989256829023361</v>
       </c>
       <c r="O21" t="n">
         <v>8</v>
@@ -1692,11 +1692,11 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>175</v>
+        <v>38</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>olive-sweep-322</t>
+          <t>dark-sweep-389</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1705,7 +1705,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>3552</v>
+        <v>1971</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
@@ -1714,12 +1714,12 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>MAnet</t>
+          <t>FPN</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>timm-regnety_120</t>
+          <t>resnet101</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1727,35 +1727,35 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>RAdam</t>
+          <t>RMSprop</t>
         </is>
       </c>
       <c r="J22" t="n">
         <v>1e-05</v>
       </c>
       <c r="K22" t="n">
-        <v>0.9890490472316742</v>
+        <v>0.9885302484035492</v>
       </c>
       <c r="L22" t="n">
-        <v>0.9784430265426636</v>
+        <v>0.9774056673049928</v>
       </c>
       <c r="M22" t="n">
-        <v>0.9903631806373596</v>
+        <v>0.9924060702323914</v>
       </c>
       <c r="N22" t="n">
-        <v>0.994059592485428</v>
+        <v>0.9880223870277404</v>
       </c>
       <c r="O22" t="n">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>51</v>
+        <v>174</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>effortless-sweep-367</t>
+          <t>wobbly-sweep-323</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1764,7 +1764,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>3394</v>
+        <v>4797</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
@@ -1773,16 +1773,16 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>PSPNet</t>
+          <t>LinkNet</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>timm-regnety_120</t>
+          <t>efficientnet-b5</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>896</v>
+        <v>640</v>
       </c>
       <c r="I23" t="inlineStr">
         <is>
@@ -1793,28 +1793,28 @@
         <v>0.0001</v>
       </c>
       <c r="K23" t="n">
-        <v>0.9876052737236024</v>
+        <v>0.9884950816631316</v>
       </c>
       <c r="L23" t="n">
-        <v>0.9755972325801848</v>
+        <v>0.9772969484329224</v>
       </c>
       <c r="M23" t="n">
-        <v>0.9946568012237548</v>
+        <v>0.9928045868873596</v>
       </c>
       <c r="N23" t="n">
-        <v>0.988731861114502</v>
+        <v>0.9911109209060668</v>
       </c>
       <c r="O23" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>321</v>
+        <v>175</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>volcanic-sweep-107</t>
+          <t>olive-sweep-322</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1823,7 +1823,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2876</v>
+        <v>3552</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -1832,16 +1832,16 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Unet</t>
+          <t>MAnet</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>resnet101</t>
+          <t>timm-regnety_120</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>768</v>
+        <v>512</v>
       </c>
       <c r="I24" t="inlineStr">
         <is>
@@ -1852,28 +1852,28 @@
         <v>1e-05</v>
       </c>
       <c r="K24" t="n">
-        <v>0.9890121817588806</v>
+        <v>0.9890490472316742</v>
       </c>
       <c r="L24" t="n">
-        <v>0.9783228933811188</v>
+        <v>0.9784430265426636</v>
       </c>
       <c r="M24" t="n">
-        <v>0.9910860955715181</v>
+        <v>0.9903631806373596</v>
       </c>
       <c r="N24" t="n">
-        <v>0.9950199723243712</v>
+        <v>0.994059592485428</v>
       </c>
       <c r="O24" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>21</v>
+        <v>389</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>desert-sweep-417</t>
+          <t>hearty-sweep-69</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1882,7 +1882,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>2965</v>
+        <v>3593</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1891,48 +1891,48 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>UnetPlusPlus</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>resnet101</t>
+          <t>efficientnet-b0</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>512</v>
+        <v>768</v>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>RMSprop</t>
+          <t>Adam</t>
         </is>
       </c>
       <c r="J25" t="n">
-        <v>1e-05</v>
+        <v>0.0001</v>
       </c>
       <c r="K25" t="n">
-        <v>0.9894071519374849</v>
+        <v>0.988418132066726</v>
       </c>
       <c r="L25" t="n">
-        <v>0.9790956676006316</v>
+        <v>0.977133482694626</v>
       </c>
       <c r="M25" t="n">
-        <v>0.9912067055702209</v>
+        <v>0.991938829421997</v>
       </c>
       <c r="N25" t="n">
-        <v>0.9928673803806304</v>
+        <v>0.989815771579742</v>
       </c>
       <c r="O25" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>302</v>
+        <v>51</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>clear-sweep-49</t>
+          <t>effortless-sweep-367</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1941,21 +1941,21 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2731</v>
+        <v>3394</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>["Vasa vasorum"]</t>
+          <t>["Lumen"]</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>DeepLabV3</t>
+          <t>PSPNet</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>resnet101</t>
+          <t>timm-regnety_120</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1963,35 +1963,35 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Adam</t>
+          <t>RAdam</t>
         </is>
       </c>
       <c r="J26" t="n">
         <v>0.0001</v>
       </c>
       <c r="K26" t="n">
-        <v>0.7194635570049286</v>
+        <v>0.9876052737236024</v>
       </c>
       <c r="L26" t="n">
-        <v>0.6174107939004898</v>
+        <v>0.9755972325801848</v>
       </c>
       <c r="M26" t="n">
-        <v>0.8410857915878296</v>
+        <v>0.9946568012237548</v>
       </c>
       <c r="N26" t="n">
-        <v>0.9078525602817537</v>
+        <v>0.988731861114502</v>
       </c>
       <c r="O26" t="n">
-        <v>37</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>220</v>
+        <v>321</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>glorious-sweep-131</t>
+          <t>volcanic-sweep-107</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2000,57 +2000,57 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>571</v>
+        <v>2876</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>["Vasa vasorum"]</t>
+          <t>["Lumen"]</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>DeepLabV3Plus</t>
+          <t>Unet</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>resnet50</t>
+          <t>resnet101</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>512</v>
+        <v>768</v>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>RMSprop</t>
+          <t>RAdam</t>
         </is>
       </c>
       <c r="J27" t="n">
-        <v>0.001</v>
+        <v>1e-05</v>
       </c>
       <c r="K27" t="n">
-        <v>0.7550063133239746</v>
+        <v>0.9890121817588806</v>
       </c>
       <c r="L27" t="n">
-        <v>0.6368829309940338</v>
+        <v>0.9783228933811188</v>
       </c>
       <c r="M27" t="n">
-        <v>0.7899507582187653</v>
+        <v>0.9910860955715181</v>
       </c>
       <c r="N27" t="n">
-        <v>0.8793827295303345</v>
+        <v>0.9950199723243712</v>
       </c>
       <c r="O27" t="n">
-        <v>43</v>
+        <v>8</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>252</v>
+        <v>21</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>polar-sweep-99</t>
+          <t>desert-sweep-417</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2059,25 +2059,25 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>2100</v>
+        <v>2965</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>["Vasa vasorum"]</t>
+          <t>["Lumen"]</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>FPN</t>
+          <t>UnetPlusPlus</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>efficientnet-b7</t>
+          <t>resnet101</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>768</v>
+        <v>512</v>
       </c>
       <c r="I28" t="inlineStr">
         <is>
@@ -2085,31 +2085,31 @@
         </is>
       </c>
       <c r="J28" t="n">
-        <v>0.0001</v>
+        <v>1e-05</v>
       </c>
       <c r="K28" t="n">
-        <v>0.7511721253395081</v>
+        <v>0.9894071519374849</v>
       </c>
       <c r="L28" t="n">
-        <v>0.6508548557758331</v>
+        <v>0.9790956676006316</v>
       </c>
       <c r="M28" t="n">
-        <v>0.874140739440918</v>
+        <v>0.9912067055702209</v>
       </c>
       <c r="N28" t="n">
-        <v>0.8207859694957733</v>
+        <v>0.9928673803806304</v>
       </c>
       <c r="O28" t="n">
-        <v>39</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>150</v>
+        <v>302</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>deep-sweep-201</t>
+          <t>clear-sweep-49</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2118,7 +2118,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1029</v>
+        <v>2731</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
@@ -2127,16 +2127,16 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>LinkNet</t>
+          <t>DeepLabV3</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>timm-regnetx_064</t>
+          <t>resnet101</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>768</v>
+        <v>896</v>
       </c>
       <c r="I29" t="inlineStr">
         <is>
@@ -2144,31 +2144,31 @@
         </is>
       </c>
       <c r="J29" t="n">
-        <v>0.001</v>
+        <v>0.0001</v>
       </c>
       <c r="K29" t="n">
-        <v>0.7577740848064423</v>
+        <v>0.7194635570049286</v>
       </c>
       <c r="L29" t="n">
-        <v>0.6430717408657074</v>
+        <v>0.6174107939004898</v>
       </c>
       <c r="M29" t="n">
-        <v>0.9020366370677948</v>
+        <v>0.8410857915878296</v>
       </c>
       <c r="N29" t="n">
-        <v>0.9285779297351836</v>
+        <v>0.9078525602817537</v>
       </c>
       <c r="O29" t="n">
-        <v>48</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>toasty-sweep-121</t>
+          <t>glorious-sweep-131</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2177,7 +2177,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>1252</v>
+        <v>571</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
@@ -2186,7 +2186,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>MAnet</t>
+          <t>DeepLabV3Plus</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2195,39 +2195,39 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>640</v>
+        <v>512</v>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>RAdam</t>
+          <t>RMSprop</t>
         </is>
       </c>
       <c r="J30" t="n">
         <v>0.001</v>
       </c>
       <c r="K30" t="n">
-        <v>0.7713472247123718</v>
+        <v>0.7550063133239746</v>
       </c>
       <c r="L30" t="n">
-        <v>0.6579388976097107</v>
+        <v>0.6368829309940338</v>
       </c>
       <c r="M30" t="n">
-        <v>0.7404732704162598</v>
+        <v>0.7899507582187653</v>
       </c>
       <c r="N30" t="n">
-        <v>1</v>
+        <v>0.8793827295303345</v>
       </c>
       <c r="O30" t="n">
-        <v>64</v>
+        <v>43</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>146</v>
+        <v>252</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>devoted-sweep-205</t>
+          <t>polar-sweep-99</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2236,7 +2236,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>1168</v>
+        <v>2100</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
@@ -2245,48 +2245,48 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>PAN</t>
+          <t>FPN</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>efficientnet-b5</t>
+          <t>efficientnet-b7</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>512</v>
+        <v>768</v>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Adam</t>
+          <t>RMSprop</t>
         </is>
       </c>
       <c r="J31" t="n">
-        <v>0.001</v>
+        <v>0.0001</v>
       </c>
       <c r="K31" t="n">
-        <v>0.7393350899219513</v>
+        <v>0.7511721253395081</v>
       </c>
       <c r="L31" t="n">
-        <v>0.6317225396633148</v>
+        <v>0.6508548557758331</v>
       </c>
       <c r="M31" t="n">
-        <v>0.8225456774234772</v>
+        <v>0.874140739440918</v>
       </c>
       <c r="N31" t="n">
-        <v>0.8181970119476318</v>
+        <v>0.8207859694957733</v>
       </c>
       <c r="O31" t="n">
-        <v>95</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>270</v>
+        <v>150</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>rose-sweep-81</t>
+          <t>deep-sweep-201</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2295,7 +2295,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>1173</v>
+        <v>1029</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
@@ -2304,48 +2304,48 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>PSPNet</t>
+          <t>LinkNet</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>timm-regnety_120</t>
+          <t>timm-regnetx_064</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>896</v>
+        <v>768</v>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>RMSprop</t>
+          <t>Adam</t>
         </is>
       </c>
       <c r="J32" t="n">
         <v>0.001</v>
       </c>
       <c r="K32" t="n">
-        <v>0.7062748074531555</v>
+        <v>0.7577740848064423</v>
       </c>
       <c r="L32" t="n">
-        <v>0.5871365368366241</v>
+        <v>0.6430717408657074</v>
       </c>
       <c r="M32" t="n">
-        <v>0.8329312801361084</v>
+        <v>0.9020366370677948</v>
       </c>
       <c r="N32" t="n">
-        <v>0.84799724817276</v>
+        <v>0.9285779297351836</v>
       </c>
       <c r="O32" t="n">
-        <v>95</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>absurd-sweep-113</t>
+          <t>toasty-sweep-121</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2354,7 +2354,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>1259</v>
+        <v>1252</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
@@ -2363,16 +2363,16 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Unet</t>
+          <t>MAnet</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>timm-regnetx_064</t>
+          <t>resnet50</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>896</v>
+        <v>640</v>
       </c>
       <c r="I33" t="inlineStr">
         <is>
@@ -2383,28 +2383,28 @@
         <v>0.001</v>
       </c>
       <c r="K33" t="n">
-        <v>0.783756285905838</v>
+        <v>0.7713472247123718</v>
       </c>
       <c r="L33" t="n">
-        <v>0.6947612166404724</v>
+        <v>0.6579388976097107</v>
       </c>
       <c r="M33" t="n">
-        <v>0.8139964044094086</v>
+        <v>0.7404732704162598</v>
       </c>
       <c r="N33" t="n">
         <v>1</v>
       </c>
       <c r="O33" t="n">
-        <v>42</v>
+        <v>64</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>25</v>
+        <v>146</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>lively-sweep-326</t>
+          <t>devoted-sweep-205</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -2413,7 +2413,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>738</v>
+        <v>1168</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
@@ -2422,12 +2422,12 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>UnetPlusPlus</t>
+          <t>PAN</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>timm-regnetx_002</t>
+          <t>efficientnet-b5</t>
         </is>
       </c>
       <c r="H34" t="n">
@@ -2442,18 +2442,195 @@
         <v>0.001</v>
       </c>
       <c r="K34" t="n">
+        <v>0.7393350899219513</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.6317225396633148</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.8225456774234772</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.8181970119476318</v>
+      </c>
+      <c r="O34" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>270</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>rose-sweep-81</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>1173</v>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>["Vasa vasorum"]</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>PSPNet</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>timm-regnety_120</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>896</v>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>RMSprop</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.7062748074531555</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.5871365368366241</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.8329312801361084</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.84799724817276</v>
+      </c>
+      <c r="O35" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>238</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>absurd-sweep-113</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>1259</v>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>["Vasa vasorum"]</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Unet</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>timm-regnetx_064</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>896</v>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>RAdam</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.783756285905838</v>
+      </c>
+      <c r="L36" t="n">
+        <v>0.6947612166404724</v>
+      </c>
+      <c r="M36" t="n">
+        <v>0.8139964044094086</v>
+      </c>
+      <c r="N36" t="n">
+        <v>1</v>
+      </c>
+      <c r="O36" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>25</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>lively-sweep-326</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>finished</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>738</v>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>["Vasa vasorum"]</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>UnetPlusPlus</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>timm-regnetx_002</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>512</v>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Adam</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="K37" t="n">
         <v>0.7592446506023407</v>
       </c>
-      <c r="L34" t="n">
+      <c r="L37" t="n">
         <v>0.6709801554679871</v>
       </c>
-      <c r="M34" t="n">
+      <c r="M37" t="n">
         <v>0.8451356887817383</v>
       </c>
-      <c r="N34" t="n">
+      <c r="N37" t="n">
         <v>0.9715909063816072</v>
       </c>
-      <c r="O34" t="n">
+      <c r="O37" t="n">
         <v>54</v>
       </c>
     </row>

</xml_diff>